<commit_message>
New: unit conversion and data file linearisation.
</commit_message>
<xml_diff>
--- a/data/zenodo_ivan/import/CHE_imp_coal.xlsx
+++ b/data/zenodo_ivan/import/CHE_imp_coal.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruiziv/switchdrive/ACCURACY/RESTORE/data/zenodo_ivan/import/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2C854C5-1E70-1A4D-B934-A028129CA2B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="38400" yWindow="-2860" windowWidth="21600" windowHeight="37900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -28,7 +34,7 @@
     <t>CHE_imp_coal.xlsx</t>
   </si>
   <si>
-    <t>2023-01-05 18:35:30</t>
+    <t>2023-01-06 14:43:57</t>
   </si>
   <si>
     <t>Ivan Ruiz Manuel</t>
@@ -214,8 +220,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -278,11 +284,19 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -324,7 +338,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -356,9 +370,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -390,6 +422,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -565,14 +615,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M275"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K33" sqref="K33"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="9" max="9" width="11.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -580,7 +635,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -588,7 +643,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -596,7 +651,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -637,7 +692,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -654,7 +709,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -671,7 +726,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -688,7 +743,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -705,7 +760,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -722,7 +777,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -739,7 +794,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -756,7 +811,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -773,7 +828,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -790,7 +845,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -807,7 +862,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -824,7 +879,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -841,7 +896,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -858,7 +913,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -875,7 +930,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -892,7 +947,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -909,7 +964,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -926,7 +981,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>19</v>
       </c>
@@ -943,7 +998,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>19</v>
       </c>
@@ -960,7 +1015,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>19</v>
       </c>
@@ -977,7 +1032,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>19</v>
       </c>
@@ -994,7 +1049,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>19</v>
       </c>
@@ -1011,7 +1066,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>19</v>
       </c>
@@ -1028,7 +1083,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>19</v>
       </c>
@@ -1045,7 +1100,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>19</v>
       </c>
@@ -1062,7 +1117,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>19</v>
       </c>
@@ -1079,7 +1134,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>19</v>
       </c>
@@ -1096,7 +1151,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>19</v>
       </c>
@@ -1113,7 +1168,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>19</v>
       </c>
@@ -1130,7 +1185,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>19</v>
       </c>
@@ -1147,7 +1202,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>19</v>
       </c>
@@ -1164,7 +1219,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>19</v>
       </c>
@@ -1181,7 +1236,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>19</v>
       </c>
@@ -1198,7 +1253,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>19</v>
       </c>
@@ -1215,7 +1270,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>19</v>
       </c>
@@ -1232,7 +1287,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>19</v>
       </c>
@@ -1249,7 +1304,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>19</v>
       </c>
@@ -1266,7 +1321,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="43" spans="1:8">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>19</v>
       </c>
@@ -1283,7 +1338,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="44" spans="1:8">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>19</v>
       </c>
@@ -1300,7 +1355,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="45" spans="1:8">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>19</v>
       </c>
@@ -1317,7 +1372,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>19</v>
       </c>
@@ -1334,7 +1389,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>19</v>
       </c>
@@ -1351,7 +1406,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>19</v>
       </c>
@@ -1368,7 +1423,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>19</v>
       </c>
@@ -1385,7 +1440,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>19</v>
       </c>
@@ -1402,7 +1457,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="51" spans="1:8">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>19</v>
       </c>
@@ -1419,7 +1474,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="52" spans="1:8">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>19</v>
       </c>
@@ -1436,7 +1491,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="53" spans="1:8">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>19</v>
       </c>
@@ -1453,7 +1508,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="54" spans="1:8">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>19</v>
       </c>
@@ -1470,7 +1525,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="55" spans="1:8">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>19</v>
       </c>
@@ -1487,7 +1542,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="56" spans="1:8">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>19</v>
       </c>
@@ -1504,7 +1559,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="57" spans="1:8">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>19</v>
       </c>
@@ -1521,7 +1576,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="58" spans="1:8">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>19</v>
       </c>
@@ -1538,7 +1593,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="59" spans="1:8">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>19</v>
       </c>
@@ -1555,7 +1610,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="60" spans="1:8">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>19</v>
       </c>
@@ -1572,7 +1627,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="61" spans="1:8">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>19</v>
       </c>
@@ -1589,7 +1644,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="62" spans="1:8">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>19</v>
       </c>
@@ -1606,7 +1661,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="63" spans="1:8">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>19</v>
       </c>
@@ -1623,7 +1678,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="64" spans="1:8">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>19</v>
       </c>
@@ -1640,7 +1695,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="65" spans="1:13">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>19</v>
       </c>
@@ -1657,7 +1712,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="66" spans="1:13">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>19</v>
       </c>
@@ -1686,7 +1741,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="67" spans="1:13">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>19</v>
       </c>
@@ -1715,7 +1770,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="68" spans="1:13">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>19</v>
       </c>
@@ -1729,7 +1784,7 @@
         <v>1992</v>
       </c>
       <c r="H68">
-        <v>90.09999999999999</v>
+        <v>90.1</v>
       </c>
       <c r="I68" t="s">
         <v>34</v>
@@ -1744,7 +1799,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="69" spans="1:13">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>19</v>
       </c>
@@ -1773,7 +1828,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="70" spans="1:13">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>19</v>
       </c>
@@ -1787,7 +1842,7 @@
         <v>1994</v>
       </c>
       <c r="H70">
-        <v>79.59999999999999</v>
+        <v>79.599999999999994</v>
       </c>
       <c r="I70" t="s">
         <v>36</v>
@@ -1802,7 +1857,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="71" spans="1:13">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>19</v>
       </c>
@@ -1831,7 +1886,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="72" spans="1:13">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>19</v>
       </c>
@@ -1860,7 +1915,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="73" spans="1:13">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>19</v>
       </c>
@@ -1889,7 +1944,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="74" spans="1:13">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>19</v>
       </c>
@@ -1918,7 +1973,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="75" spans="1:13">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>19</v>
       </c>
@@ -1947,7 +2002,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="76" spans="1:13">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>19</v>
       </c>
@@ -1961,7 +2016,7 @@
         <v>2000</v>
       </c>
       <c r="H76">
-        <v>85.90000000000001</v>
+        <v>85.9</v>
       </c>
       <c r="I76" t="s">
         <v>42</v>
@@ -1976,7 +2031,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="77" spans="1:13">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>19</v>
       </c>
@@ -1990,7 +2045,7 @@
         <v>2001</v>
       </c>
       <c r="H77">
-        <v>98.09999999999999</v>
+        <v>98.1</v>
       </c>
       <c r="I77" t="s">
         <v>43</v>
@@ -2005,7 +2060,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="78" spans="1:13">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>19</v>
       </c>
@@ -2019,7 +2074,7 @@
         <v>2002</v>
       </c>
       <c r="H78">
-        <v>88.09999999999999</v>
+        <v>88.1</v>
       </c>
       <c r="I78" t="s">
         <v>44</v>
@@ -2034,7 +2089,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="79" spans="1:13">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>19</v>
       </c>
@@ -2063,7 +2118,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="80" spans="1:13">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>19</v>
       </c>
@@ -2077,7 +2132,7 @@
         <v>2004</v>
       </c>
       <c r="H80">
-        <v>157.3</v>
+        <v>157.30000000000001</v>
       </c>
       <c r="I80" t="s">
         <v>46</v>
@@ -2092,7 +2147,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="81" spans="1:13">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>19</v>
       </c>
@@ -2106,7 +2161,7 @@
         <v>2005</v>
       </c>
       <c r="H81">
-        <v>157.2</v>
+        <v>157.19999999999999</v>
       </c>
       <c r="I81" t="s">
         <v>47</v>
@@ -2121,7 +2176,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="82" spans="1:13">
+    <row r="82" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>19</v>
       </c>
@@ -2150,7 +2205,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="83" spans="1:13">
+    <row r="83" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>19</v>
       </c>
@@ -2179,7 +2234,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="84" spans="1:13">
+    <row r="84" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>19</v>
       </c>
@@ -2208,7 +2263,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="85" spans="1:13">
+    <row r="85" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>19</v>
       </c>
@@ -2237,7 +2292,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="86" spans="1:13">
+    <row r="86" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>19</v>
       </c>
@@ -2251,7 +2306,7 @@
         <v>2010</v>
       </c>
       <c r="H86">
-        <v>258.9</v>
+        <v>258.89999999999998</v>
       </c>
       <c r="I86" t="s">
         <v>52</v>
@@ -2266,7 +2321,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="87" spans="1:13">
+    <row r="87" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>19</v>
       </c>
@@ -2295,7 +2350,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="88" spans="1:13">
+    <row r="88" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>19</v>
       </c>
@@ -2324,7 +2379,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="89" spans="1:13">
+    <row r="89" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>19</v>
       </c>
@@ -2353,7 +2408,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="90" spans="1:13">
+    <row r="90" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>19</v>
       </c>
@@ -2382,7 +2437,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="91" spans="1:13">
+    <row r="91" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>19</v>
       </c>
@@ -2411,7 +2466,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="92" spans="1:13">
+    <row r="92" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>19</v>
       </c>
@@ -2440,7 +2495,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="93" spans="1:13">
+    <row r="93" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>19</v>
       </c>
@@ -2469,7 +2524,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="94" spans="1:13">
+    <row r="94" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>19</v>
       </c>
@@ -2498,7 +2553,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="95" spans="1:13">
+    <row r="95" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>19</v>
       </c>
@@ -2527,7 +2582,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="96" spans="1:13">
+    <row r="96" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>19</v>
       </c>
@@ -2544,7 +2599,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:8">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>19</v>
       </c>
@@ -2561,7 +2616,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:8">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>19</v>
       </c>
@@ -2578,7 +2633,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:8">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>19</v>
       </c>
@@ -2595,7 +2650,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:8">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>19</v>
       </c>
@@ -2612,7 +2667,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:8">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>19</v>
       </c>
@@ -2629,7 +2684,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:8">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>19</v>
       </c>
@@ -2646,7 +2701,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:8">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>19</v>
       </c>
@@ -2663,7 +2718,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:8">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>19</v>
       </c>
@@ -2680,7 +2735,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:8">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>19</v>
       </c>
@@ -2697,7 +2752,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:8">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>19</v>
       </c>
@@ -2714,7 +2769,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:8">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>19</v>
       </c>
@@ -2731,7 +2786,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:8">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>19</v>
       </c>
@@ -2748,7 +2803,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:8">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>19</v>
       </c>
@@ -2765,7 +2820,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:8">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>19</v>
       </c>
@@ -2782,7 +2837,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:8">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>19</v>
       </c>
@@ -2799,7 +2854,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:8">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>19</v>
       </c>
@@ -2816,7 +2871,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:8">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>19</v>
       </c>
@@ -2833,7 +2888,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:8">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>19</v>
       </c>
@@ -2850,7 +2905,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:8">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>19</v>
       </c>
@@ -2867,7 +2922,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:8">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>19</v>
       </c>
@@ -2884,7 +2939,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:8">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>19</v>
       </c>
@@ -2901,7 +2956,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:8">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>19</v>
       </c>
@@ -2918,7 +2973,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:8">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>19</v>
       </c>
@@ -2935,7 +2990,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:8">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>19</v>
       </c>
@@ -2952,7 +3007,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:8">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>19</v>
       </c>
@@ -2969,7 +3024,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:8">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>19</v>
       </c>
@@ -2986,7 +3041,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:8">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>19</v>
       </c>
@@ -3003,7 +3058,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:8">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>19</v>
       </c>
@@ -3020,7 +3075,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="1:8">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>19</v>
       </c>
@@ -3037,7 +3092,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="1:8">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>19</v>
       </c>
@@ -3054,7 +3109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:8">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>19</v>
       </c>
@@ -3071,7 +3126,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:8">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>19</v>
       </c>
@@ -3088,7 +3143,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:8">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>19</v>
       </c>
@@ -3105,7 +3160,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:8">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>19</v>
       </c>
@@ -3122,7 +3177,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:8">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>19</v>
       </c>
@@ -3139,7 +3194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:8">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>19</v>
       </c>
@@ -3156,7 +3211,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:8">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>19</v>
       </c>
@@ -3173,7 +3228,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:8">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>19</v>
       </c>
@@ -3190,7 +3245,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:8">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>19</v>
       </c>
@@ -3207,7 +3262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:8">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>19</v>
       </c>
@@ -3224,7 +3279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:8">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>19</v>
       </c>
@@ -3241,7 +3296,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:8">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>19</v>
       </c>
@@ -3258,7 +3313,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:8">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>19</v>
       </c>
@@ -3275,7 +3330,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:8">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>19</v>
       </c>
@@ -3292,7 +3347,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:8">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>19</v>
       </c>
@@ -3309,7 +3364,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:8">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>19</v>
       </c>
@@ -3326,7 +3381,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:8">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>19</v>
       </c>
@@ -3343,7 +3398,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:8">
+    <row r="144" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>19</v>
       </c>
@@ -3360,7 +3415,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:8">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>19</v>
       </c>
@@ -3377,7 +3432,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:8">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>19</v>
       </c>
@@ -3394,7 +3449,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:8">
+    <row r="147" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>19</v>
       </c>
@@ -3411,7 +3466,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:8">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>19</v>
       </c>
@@ -3428,7 +3483,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:8">
+    <row r="149" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>19</v>
       </c>
@@ -3445,7 +3500,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:8">
+    <row r="150" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>19</v>
       </c>
@@ -3462,7 +3517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:8">
+    <row r="151" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>19</v>
       </c>
@@ -3479,7 +3534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:8">
+    <row r="152" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>19</v>
       </c>
@@ -3496,7 +3551,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:8">
+    <row r="153" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>19</v>
       </c>
@@ -3513,7 +3568,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:8">
+    <row r="154" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>19</v>
       </c>
@@ -3530,7 +3585,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:8">
+    <row r="155" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>19</v>
       </c>
@@ -3547,7 +3602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:8">
+    <row r="156" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>19</v>
       </c>
@@ -3564,7 +3619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:8">
+    <row r="157" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>19</v>
       </c>
@@ -3581,7 +3636,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:8">
+    <row r="158" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>19</v>
       </c>
@@ -3598,7 +3653,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:8">
+    <row r="159" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>19</v>
       </c>
@@ -3615,7 +3670,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:8">
+    <row r="160" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>19</v>
       </c>
@@ -3632,7 +3687,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:8">
+    <row r="161" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>19</v>
       </c>
@@ -3649,7 +3704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:8">
+    <row r="162" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>19</v>
       </c>
@@ -3666,7 +3721,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:8">
+    <row r="163" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>19</v>
       </c>
@@ -3683,7 +3738,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:8">
+    <row r="164" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>19</v>
       </c>
@@ -3700,7 +3755,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:8">
+    <row r="165" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>19</v>
       </c>
@@ -3717,7 +3772,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:8">
+    <row r="166" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>19</v>
       </c>
@@ -3734,7 +3789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:8">
+    <row r="167" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>19</v>
       </c>
@@ -3751,7 +3806,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:8">
+    <row r="168" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>19</v>
       </c>
@@ -3768,7 +3823,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:8">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>19</v>
       </c>
@@ -3785,7 +3840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:8">
+    <row r="170" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>19</v>
       </c>
@@ -3802,7 +3857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:8">
+    <row r="171" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>19</v>
       </c>
@@ -3819,7 +3874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="1:8">
+    <row r="172" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>19</v>
       </c>
@@ -3836,7 +3891,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="1:8">
+    <row r="173" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>19</v>
       </c>
@@ -3853,7 +3908,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:8">
+    <row r="174" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>19</v>
       </c>
@@ -3870,7 +3925,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:8">
+    <row r="175" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>19</v>
       </c>
@@ -3887,7 +3942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:8">
+    <row r="176" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>19</v>
       </c>
@@ -3904,7 +3959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:8">
+    <row r="177" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>19</v>
       </c>
@@ -3921,7 +3976,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="1:8">
+    <row r="178" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>19</v>
       </c>
@@ -3938,7 +3993,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="1:8">
+    <row r="179" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>19</v>
       </c>
@@ -3955,7 +4010,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="1:8">
+    <row r="180" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>19</v>
       </c>
@@ -3972,7 +4027,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="1:8">
+    <row r="181" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>19</v>
       </c>
@@ -3989,7 +4044,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="182" spans="1:8">
+    <row r="182" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>19</v>
       </c>
@@ -4006,7 +4061,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="183" spans="1:8">
+    <row r="183" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>19</v>
       </c>
@@ -4023,7 +4078,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="1:8">
+    <row r="184" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>19</v>
       </c>
@@ -4040,7 +4095,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:8">
+    <row r="185" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>19</v>
       </c>
@@ -4057,7 +4112,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="186" spans="1:8">
+    <row r="186" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>19</v>
       </c>
@@ -4074,7 +4129,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="187" spans="1:8">
+    <row r="187" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>19</v>
       </c>
@@ -4091,7 +4146,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="188" spans="1:8">
+    <row r="188" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>19</v>
       </c>
@@ -4108,7 +4163,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="189" spans="1:8">
+    <row r="189" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>19</v>
       </c>
@@ -4125,7 +4180,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="190" spans="1:8">
+    <row r="190" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>19</v>
       </c>
@@ -4142,7 +4197,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="191" spans="1:8">
+    <row r="191" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>19</v>
       </c>
@@ -4159,7 +4214,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="192" spans="1:8">
+    <row r="192" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>19</v>
       </c>
@@ -4176,7 +4231,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="193" spans="1:8">
+    <row r="193" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>19</v>
       </c>
@@ -4193,7 +4248,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="194" spans="1:8">
+    <row r="194" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>19</v>
       </c>
@@ -4210,7 +4265,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="195" spans="1:8">
+    <row r="195" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>19</v>
       </c>
@@ -4227,7 +4282,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="196" spans="1:8">
+    <row r="196" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>19</v>
       </c>
@@ -4244,7 +4299,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="197" spans="1:8">
+    <row r="197" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>19</v>
       </c>
@@ -4261,7 +4316,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="198" spans="1:8">
+    <row r="198" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>19</v>
       </c>
@@ -4278,7 +4333,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="199" spans="1:8">
+    <row r="199" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>19</v>
       </c>
@@ -4295,7 +4350,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="200" spans="1:8">
+    <row r="200" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>19</v>
       </c>
@@ -4312,7 +4367,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="201" spans="1:8">
+    <row r="201" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>19</v>
       </c>
@@ -4329,7 +4384,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="202" spans="1:8">
+    <row r="202" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>19</v>
       </c>
@@ -4346,7 +4401,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="203" spans="1:8">
+    <row r="203" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>19</v>
       </c>
@@ -4363,7 +4418,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="204" spans="1:8">
+    <row r="204" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>19</v>
       </c>
@@ -4380,7 +4435,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="205" spans="1:8">
+    <row r="205" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>19</v>
       </c>
@@ -4397,7 +4452,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="206" spans="1:8">
+    <row r="206" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
         <v>19</v>
       </c>
@@ -4414,7 +4469,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="207" spans="1:8">
+    <row r="207" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>19</v>
       </c>
@@ -4431,7 +4486,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="208" spans="1:8">
+    <row r="208" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>19</v>
       </c>
@@ -4448,7 +4503,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="209" spans="1:8">
+    <row r="209" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
         <v>19</v>
       </c>
@@ -4465,7 +4520,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="210" spans="1:8">
+    <row r="210" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
         <v>19</v>
       </c>
@@ -4482,7 +4537,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="211" spans="1:8">
+    <row r="211" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
         <v>19</v>
       </c>
@@ -4499,7 +4554,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="212" spans="1:8">
+    <row r="212" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
         <v>19</v>
       </c>
@@ -4516,7 +4571,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="213" spans="1:8">
+    <row r="213" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
         <v>19</v>
       </c>
@@ -4533,7 +4588,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="214" spans="1:8">
+    <row r="214" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
         <v>19</v>
       </c>
@@ -4550,7 +4605,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="215" spans="1:8">
+    <row r="215" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
         <v>19</v>
       </c>
@@ -4567,7 +4622,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="216" spans="1:8">
+    <row r="216" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
         <v>19</v>
       </c>
@@ -4584,7 +4639,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="217" spans="1:8">
+    <row r="217" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
         <v>19</v>
       </c>
@@ -4601,7 +4656,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="218" spans="1:8">
+    <row r="218" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
         <v>19</v>
       </c>
@@ -4618,7 +4673,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="219" spans="1:8">
+    <row r="219" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
         <v>19</v>
       </c>
@@ -4635,7 +4690,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="220" spans="1:8">
+    <row r="220" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
         <v>19</v>
       </c>
@@ -4652,7 +4707,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="221" spans="1:8">
+    <row r="221" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
         <v>19</v>
       </c>
@@ -4669,7 +4724,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="222" spans="1:8">
+    <row r="222" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
         <v>19</v>
       </c>
@@ -4686,7 +4741,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="223" spans="1:8">
+    <row r="223" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
         <v>19</v>
       </c>
@@ -4703,7 +4758,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="224" spans="1:8">
+    <row r="224" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
         <v>19</v>
       </c>
@@ -4720,7 +4775,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="225" spans="1:8">
+    <row r="225" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
         <v>19</v>
       </c>
@@ -4737,7 +4792,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="226" spans="1:8">
+    <row r="226" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
         <v>19</v>
       </c>
@@ -4754,7 +4809,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="227" spans="1:8">
+    <row r="227" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
         <v>19</v>
       </c>
@@ -4771,7 +4826,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="228" spans="1:8">
+    <row r="228" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
         <v>19</v>
       </c>
@@ -4788,7 +4843,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="229" spans="1:8">
+    <row r="229" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
         <v>19</v>
       </c>
@@ -4805,7 +4860,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="230" spans="1:8">
+    <row r="230" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
         <v>19</v>
       </c>
@@ -4822,7 +4877,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="231" spans="1:8">
+    <row r="231" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
         <v>19</v>
       </c>
@@ -4839,7 +4894,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="232" spans="1:8">
+    <row r="232" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
         <v>19</v>
       </c>
@@ -4856,7 +4911,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="233" spans="1:8">
+    <row r="233" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
         <v>19</v>
       </c>
@@ -4873,7 +4928,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="234" spans="1:8">
+    <row r="234" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
         <v>19</v>
       </c>
@@ -4890,7 +4945,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="235" spans="1:8">
+    <row r="235" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
         <v>19</v>
       </c>
@@ -4907,7 +4962,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="236" spans="1:8">
+    <row r="236" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
         <v>19</v>
       </c>
@@ -4924,7 +4979,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="237" spans="1:8">
+    <row r="237" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
         <v>19</v>
       </c>
@@ -4941,7 +4996,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="238" spans="1:8">
+    <row r="238" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
         <v>19</v>
       </c>
@@ -4958,7 +5013,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="239" spans="1:8">
+    <row r="239" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
         <v>19</v>
       </c>
@@ -4975,7 +5030,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="240" spans="1:8">
+    <row r="240" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
         <v>19</v>
       </c>
@@ -4992,7 +5047,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="241" spans="1:8">
+    <row r="241" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
         <v>19</v>
       </c>
@@ -5009,7 +5064,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="242" spans="1:8">
+    <row r="242" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
         <v>19</v>
       </c>
@@ -5026,7 +5081,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="243" spans="1:8">
+    <row r="243" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
         <v>19</v>
       </c>
@@ -5043,7 +5098,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="244" spans="1:8">
+    <row r="244" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
         <v>19</v>
       </c>
@@ -5060,7 +5115,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="245" spans="1:8">
+    <row r="245" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
         <v>19</v>
       </c>
@@ -5077,7 +5132,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="246" spans="1:8">
+    <row r="246" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
         <v>19</v>
       </c>
@@ -5094,7 +5149,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="247" spans="1:8">
+    <row r="247" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
         <v>19</v>
       </c>
@@ -5111,7 +5166,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="248" spans="1:8">
+    <row r="248" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
         <v>19</v>
       </c>
@@ -5128,7 +5183,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="249" spans="1:8">
+    <row r="249" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
         <v>19</v>
       </c>
@@ -5145,7 +5200,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="250" spans="1:8">
+    <row r="250" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
         <v>19</v>
       </c>
@@ -5162,7 +5217,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="251" spans="1:8">
+    <row r="251" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
         <v>19</v>
       </c>
@@ -5179,7 +5234,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="252" spans="1:8">
+    <row r="252" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
         <v>19</v>
       </c>
@@ -5196,7 +5251,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="253" spans="1:8">
+    <row r="253" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
         <v>19</v>
       </c>
@@ -5213,7 +5268,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="254" spans="1:8">
+    <row r="254" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
         <v>19</v>
       </c>
@@ -5230,7 +5285,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="255" spans="1:8">
+    <row r="255" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
         <v>19</v>
       </c>
@@ -5247,7 +5302,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="256" spans="1:8">
+    <row r="256" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
         <v>19</v>
       </c>
@@ -5264,7 +5319,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="257" spans="1:8">
+    <row r="257" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
         <v>19</v>
       </c>
@@ -5281,7 +5336,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="258" spans="1:8">
+    <row r="258" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
         <v>19</v>
       </c>
@@ -5298,7 +5353,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="259" spans="1:8">
+    <row r="259" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
         <v>19</v>
       </c>
@@ -5315,7 +5370,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="260" spans="1:8">
+    <row r="260" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
         <v>19</v>
       </c>
@@ -5332,7 +5387,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="261" spans="1:8">
+    <row r="261" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
         <v>19</v>
       </c>
@@ -5349,7 +5404,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="262" spans="1:8">
+    <row r="262" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
         <v>19</v>
       </c>
@@ -5366,7 +5421,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="263" spans="1:8">
+    <row r="263" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A263" t="s">
         <v>19</v>
       </c>
@@ -5383,7 +5438,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="264" spans="1:8">
+    <row r="264" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A264" t="s">
         <v>19</v>
       </c>
@@ -5400,7 +5455,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="265" spans="1:8">
+    <row r="265" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A265" t="s">
         <v>19</v>
       </c>
@@ -5417,7 +5472,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="266" spans="1:8">
+    <row r="266" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A266" t="s">
         <v>19</v>
       </c>
@@ -5434,7 +5489,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="267" spans="1:8">
+    <row r="267" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A267" t="s">
         <v>19</v>
       </c>
@@ -5451,7 +5506,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="268" spans="1:8">
+    <row r="268" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A268" t="s">
         <v>19</v>
       </c>
@@ -5468,7 +5523,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="269" spans="1:8">
+    <row r="269" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A269" t="s">
         <v>19</v>
       </c>
@@ -5485,7 +5540,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="270" spans="1:8">
+    <row r="270" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A270" t="s">
         <v>19</v>
       </c>
@@ -5502,7 +5557,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="271" spans="1:8">
+    <row r="271" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A271" t="s">
         <v>19</v>
       </c>
@@ -5519,7 +5574,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="272" spans="1:8">
+    <row r="272" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A272" t="s">
         <v>19</v>
       </c>
@@ -5536,7 +5591,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="273" spans="1:8">
+    <row r="273" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A273" t="s">
         <v>19</v>
       </c>
@@ -5553,7 +5608,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="274" spans="1:8">
+    <row r="274" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A274" t="s">
         <v>19</v>
       </c>
@@ -5570,7 +5625,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="275" spans="1:8">
+    <row r="275" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A275" t="s">
         <v>19</v>
       </c>

</xml_diff>